<commit_message>
delete row is working.
</commit_message>
<xml_diff>
--- a/FloorLocation/FLOOR_LOCATION.xlsx
+++ b/FloorLocation/FLOOR_LOCATION.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="150">
   <si>
     <t>LOCATION_NAME</t>
   </si>
@@ -470,12 +470,6 @@
   </si>
   <si>
     <t>1</t>
-  </si>
-  <si>
-    <t>HEINZ58</t>
-  </si>
-  <si>
-    <t>2</t>
   </si>
 </sst>
 </file>
@@ -1317,7 +1311,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C148"/>
+  <dimension ref="A1:C147"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
       <selection activeCell="A147" sqref="A147"/>
@@ -2947,17 +2941,6 @@
         <v>23</v>
       </c>
     </row>
-    <row r="148">
-      <c r="A148" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="B148" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="C148" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Fixed the pageCount rounding up
</commit_message>
<xml_diff>
--- a/FloorLocation/FLOOR_LOCATION.xlsx
+++ b/FloorLocation/FLOOR_LOCATION.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="152">
   <si>
     <t>LOCATION_NAME</t>
   </si>
@@ -470,6 +470,12 @@
   </si>
   <si>
     <t>99</t>
+  </si>
+  <si>
+    <t>BUBBLEUP</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -1311,7 +1317,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C146"/>
+  <dimension ref="A1:C147"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
       <selection activeCell="A147" sqref="A147"/>
@@ -2930,6 +2936,17 @@
         <v>24</v>
       </c>
     </row>
+    <row r="147">
+      <c r="A147" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B147" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="C147" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
All paths return to correct page numbe
</commit_message>
<xml_diff>
--- a/FloorLocation/FLOOR_LOCATION.xlsx
+++ b/FloorLocation/FLOOR_LOCATION.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
   <si>
     <t>LOCATION_NAME</t>
   </si>
@@ -475,7 +475,19 @@
     <t>BUBBLEUP</t>
   </si>
   <si>
-    <t>3</t>
+    <t>30</t>
+  </si>
+  <si>
+    <t>WD40</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>ROCK</t>
+  </si>
+  <si>
+    <t>PAPER</t>
   </si>
 </sst>
 </file>
@@ -1317,7 +1329,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C147"/>
+  <dimension ref="A1:C149"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
       <selection activeCell="A147" sqref="A147"/>
@@ -2947,6 +2959,28 @@
         <v>24</v>
       </c>
     </row>
+    <row r="148">
+      <c r="A148" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B148" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="C148" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B149" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="C149" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
delete api and javascript are done
Need to add page size as a parameter to the javascript functions
</commit_message>
<xml_diff>
--- a/FloorLocation/FLOOR_LOCATION.xlsx
+++ b/FloorLocation/FLOOR_LOCATION.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlolsen/projects/FloorLocation/FloorLocation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{051E6817-64DF-D246-9847-1BD42554879C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A9F1F6-BF84-8243-A4AF-C98B353F3CB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="154">
   <si>
     <t>LOCATION_NAME</t>
   </si>
@@ -482,12 +482,6 @@
   </si>
   <si>
     <t>40</t>
-  </si>
-  <si>
-    <t>ROCK</t>
-  </si>
-  <si>
-    <t>PAPER</t>
   </si>
 </sst>
 </file>
@@ -1329,10 +1323,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C149"/>
+  <dimension ref="A1:C148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="A147" sqref="A147"/>
+    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="C149" sqref="C149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2970,17 +2964,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="149">
-      <c r="A149" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="B149" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="C149" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
added update to api
</commit_message>
<xml_diff>
--- a/FloorLocation/FLOOR_LOCATION.xlsx
+++ b/FloorLocation/FLOOR_LOCATION.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlolsen/projects/FloorLocation/FloorLocation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A9F1F6-BF84-8243-A4AF-C98B353F3CB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22337DED-2048-884D-8859-4E05BA3F16DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="155">
   <si>
     <t>LOCATION_NAME</t>
   </si>
@@ -34,15 +34,18 @@
     <t>10B</t>
   </si>
   <si>
-    <t>1</t>
+    <t>99</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>10C</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
-    <t>10C</t>
-  </si>
-  <si>
     <t>10D</t>
   </si>
   <si>
@@ -94,9 +97,6 @@
     <t>12D</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>12E</t>
   </si>
   <si>
@@ -469,9 +469,6 @@
     <t>HEINZ57</t>
   </si>
   <si>
-    <t>99</t>
-  </si>
-  <si>
     <t>BUBBLEUP</t>
   </si>
   <si>
@@ -482,6 +479,12 @@
   </si>
   <si>
     <t>40</t>
+  </si>
+  <si>
+    <t>ROCK</t>
+  </si>
+  <si>
+    <t>PAPER</t>
   </si>
 </sst>
 </file>
@@ -1323,10 +1326,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C148"/>
+  <dimension ref="A1:C149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
-      <selection activeCell="C149" sqref="C149"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1366,194 +1369,194 @@
         <v>1</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="0">
         <v>1</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="0">
         <v>1</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="0">
         <v>1</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" s="0">
         <v>1</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="0">
         <v>1</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="0">
         <v>1</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" s="0">
         <v>1</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11" s="0">
         <v>1</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" s="0">
         <v>1</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B13" s="0">
         <v>1</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B14" s="0">
         <v>1</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B15" s="0">
         <v>1</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B16" s="0">
         <v>1</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B17" s="0">
         <v>1</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B18" s="0">
         <v>1</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B19" s="0">
         <v>1</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B20" s="0">
         <v>1</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21">
@@ -1564,7 +1567,7 @@
         <v>1</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22">
@@ -1575,7 +1578,7 @@
         <v>1</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23">
@@ -1586,7 +1589,7 @@
         <v>1</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24">
@@ -1597,7 +1600,7 @@
         <v>1</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25">
@@ -1608,7 +1611,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26">
@@ -1619,7 +1622,7 @@
         <v>1</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27">
@@ -1630,7 +1633,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28">
@@ -1641,7 +1644,7 @@
         <v>1</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29">
@@ -1652,7 +1655,7 @@
         <v>1</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30">
@@ -1663,7 +1666,7 @@
         <v>1</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31">
@@ -1674,7 +1677,7 @@
         <v>1</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32">
@@ -1685,7 +1688,7 @@
         <v>1</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33">
@@ -1696,7 +1699,7 @@
         <v>1</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34">
@@ -1707,7 +1710,7 @@
         <v>1</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35">
@@ -1718,7 +1721,7 @@
         <v>1</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36">
@@ -1729,7 +1732,7 @@
         <v>1</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37">
@@ -1740,7 +1743,7 @@
         <v>1</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38">
@@ -1751,7 +1754,7 @@
         <v>1</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39">
@@ -1762,7 +1765,7 @@
         <v>1</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40">
@@ -1773,7 +1776,7 @@
         <v>1</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41">
@@ -1784,7 +1787,7 @@
         <v>1</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42">
@@ -1795,7 +1798,7 @@
         <v>1</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43">
@@ -1806,7 +1809,7 @@
         <v>1</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44">
@@ -1817,7 +1820,7 @@
         <v>1</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45">
@@ -1828,7 +1831,7 @@
         <v>1</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46">
@@ -1839,7 +1842,7 @@
         <v>1</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47">
@@ -1850,7 +1853,7 @@
         <v>1</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48">
@@ -1861,7 +1864,7 @@
         <v>1</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49">
@@ -1872,7 +1875,7 @@
         <v>1</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50">
@@ -1883,7 +1886,7 @@
         <v>1</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51">
@@ -1894,7 +1897,7 @@
         <v>1</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52">
@@ -1905,7 +1908,7 @@
         <v>1</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53">
@@ -1916,7 +1919,7 @@
         <v>1</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="54">
@@ -1927,7 +1930,7 @@
         <v>1</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55">
@@ -1938,7 +1941,7 @@
         <v>1</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56">
@@ -1949,7 +1952,7 @@
         <v>1</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57">
@@ -1960,7 +1963,7 @@
         <v>1</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="58">
@@ -1971,7 +1974,7 @@
         <v>1</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="59">
@@ -1982,7 +1985,7 @@
         <v>1</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60">
@@ -1993,7 +1996,7 @@
         <v>1</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61">
@@ -2004,7 +2007,7 @@
         <v>1</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="62">
@@ -2015,7 +2018,7 @@
         <v>1</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="63">
@@ -2026,7 +2029,7 @@
         <v>1</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="64">
@@ -2037,7 +2040,7 @@
         <v>1</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="65">
@@ -2048,7 +2051,7 @@
         <v>1</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="66">
@@ -2059,7 +2062,7 @@
         <v>1</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67">
@@ -2070,7 +2073,7 @@
         <v>1</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="68">
@@ -2081,7 +2084,7 @@
         <v>1</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="69">
@@ -2092,7 +2095,7 @@
         <v>1</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="70">
@@ -2103,7 +2106,7 @@
         <v>1</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="71">
@@ -2114,7 +2117,7 @@
         <v>1</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="72">
@@ -2125,7 +2128,7 @@
         <v>1</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="73">
@@ -2136,7 +2139,7 @@
         <v>1</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="74">
@@ -2147,7 +2150,7 @@
         <v>1</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="75">
@@ -2158,7 +2161,7 @@
         <v>1</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="76">
@@ -2169,7 +2172,7 @@
         <v>1</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="77">
@@ -2180,7 +2183,7 @@
         <v>1</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="78">
@@ -2191,7 +2194,7 @@
         <v>1</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="79">
@@ -2202,7 +2205,7 @@
         <v>1</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="80">
@@ -2213,7 +2216,7 @@
         <v>1</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="81">
@@ -2224,7 +2227,7 @@
         <v>1</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="82">
@@ -2235,7 +2238,7 @@
         <v>1</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="83">
@@ -2246,7 +2249,7 @@
         <v>1</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="84">
@@ -2257,7 +2260,7 @@
         <v>1</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="85">
@@ -2268,7 +2271,7 @@
         <v>1</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="86">
@@ -2279,7 +2282,7 @@
         <v>1</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="87">
@@ -2290,7 +2293,7 @@
         <v>1</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="88">
@@ -2301,7 +2304,7 @@
         <v>1</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="89">
@@ -2312,7 +2315,7 @@
         <v>1</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="90">
@@ -2323,7 +2326,7 @@
         <v>1</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="91">
@@ -2334,7 +2337,7 @@
         <v>1</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="92">
@@ -2345,7 +2348,7 @@
         <v>1</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="93">
@@ -2356,7 +2359,7 @@
         <v>1</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="94">
@@ -2367,7 +2370,7 @@
         <v>1</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="95">
@@ -2378,7 +2381,7 @@
         <v>1</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="96">
@@ -2389,7 +2392,7 @@
         <v>1</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="97">
@@ -2400,7 +2403,7 @@
         <v>1</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="98">
@@ -2411,7 +2414,7 @@
         <v>1</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="99">
@@ -2422,7 +2425,7 @@
         <v>1</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="100">
@@ -2433,7 +2436,7 @@
         <v>1</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="101">
@@ -2444,7 +2447,7 @@
         <v>1</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="102">
@@ -2455,7 +2458,7 @@
         <v>1</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="103">
@@ -2466,7 +2469,7 @@
         <v>1</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="104">
@@ -2477,7 +2480,7 @@
         <v>1</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="105">
@@ -2488,7 +2491,7 @@
         <v>1</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="106">
@@ -2499,7 +2502,7 @@
         <v>1</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="107">
@@ -2510,7 +2513,7 @@
         <v>1</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="108">
@@ -2521,7 +2524,7 @@
         <v>1</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="109">
@@ -2532,7 +2535,7 @@
         <v>1</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="110">
@@ -2543,7 +2546,7 @@
         <v>1</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="111">
@@ -2554,7 +2557,7 @@
         <v>1</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="112">
@@ -2565,7 +2568,7 @@
         <v>1</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="113">
@@ -2576,7 +2579,7 @@
         <v>1</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="114">
@@ -2587,7 +2590,7 @@
         <v>1</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="115">
@@ -2598,7 +2601,7 @@
         <v>1</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="116">
@@ -2609,7 +2612,7 @@
         <v>1</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="117">
@@ -2620,7 +2623,7 @@
         <v>1</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="118">
@@ -2631,7 +2634,7 @@
         <v>1</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="119">
@@ -2642,7 +2645,7 @@
         <v>1</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="120">
@@ -2653,7 +2656,7 @@
         <v>1</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="121">
@@ -2664,7 +2667,7 @@
         <v>1</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="122">
@@ -2675,7 +2678,7 @@
         <v>1</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="123">
@@ -2686,7 +2689,7 @@
         <v>1</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="124">
@@ -2697,7 +2700,7 @@
         <v>1</v>
       </c>
       <c r="C124" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="125">
@@ -2708,7 +2711,7 @@
         <v>1</v>
       </c>
       <c r="C125" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="126">
@@ -2719,7 +2722,7 @@
         <v>1</v>
       </c>
       <c r="C126" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="127">
@@ -2730,7 +2733,7 @@
         <v>1</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="128">
@@ -2741,7 +2744,7 @@
         <v>1</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="129">
@@ -2752,7 +2755,7 @@
         <v>1</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="130">
@@ -2763,7 +2766,7 @@
         <v>1</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="131">
@@ -2774,7 +2777,7 @@
         <v>1</v>
       </c>
       <c r="C131" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="132">
@@ -2785,7 +2788,7 @@
         <v>1</v>
       </c>
       <c r="C132" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="133">
@@ -2796,7 +2799,7 @@
         <v>1</v>
       </c>
       <c r="C133" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="134">
@@ -2807,7 +2810,7 @@
         <v>1</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="135">
@@ -2818,7 +2821,7 @@
         <v>1</v>
       </c>
       <c r="C135" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="136">
@@ -2829,7 +2832,7 @@
         <v>1</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="137">
@@ -2840,7 +2843,7 @@
         <v>1</v>
       </c>
       <c r="C137" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="138">
@@ -2851,7 +2854,7 @@
         <v>1</v>
       </c>
       <c r="C138" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="139">
@@ -2862,7 +2865,7 @@
         <v>1</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="140">
@@ -2873,7 +2876,7 @@
         <v>1</v>
       </c>
       <c r="C140" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="141">
@@ -2884,7 +2887,7 @@
         <v>1</v>
       </c>
       <c r="C141" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="142">
@@ -2895,7 +2898,7 @@
         <v>1</v>
       </c>
       <c r="C142" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="143">
@@ -2906,7 +2909,7 @@
         <v>1</v>
       </c>
       <c r="C143" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="144">
@@ -2917,7 +2920,7 @@
         <v>1</v>
       </c>
       <c r="C144" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="145">
@@ -2928,7 +2931,7 @@
         <v>1</v>
       </c>
       <c r="C145" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="146">
@@ -2936,31 +2939,42 @@
         <v>148</v>
       </c>
       <c r="B146" s="0" t="s">
-        <v>149</v>
+        <v>4</v>
       </c>
       <c r="C146" s="0" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B147" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="B147" s="0" t="s">
-        <v>151</v>
-      </c>
       <c r="C147" s="0" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B148" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="B148" s="0" t="s">
+      <c r="C148" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="C148" s="0" t="s">
+      <c r="B149" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="C149" s="0" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>